<commit_message>
add 14 buttons and 28 pipes in resources
</commit_message>
<xml_diff>
--- a/bird demo/Art & Sound Resources.xlsx
+++ b/bird demo/Art & Sound Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkggbo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alicejuan/Documents/03_UK/07_UoB/TB2/02_software_engineering/course_work_game/2024-group-11/bird demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC82F56C-C489-40E6-AFB2-14B427E168D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EED11BE-7AEA-4348-8954-0408F16FAA22}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
   <si>
     <t>red</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -200,30 +200,58 @@
     <t>4Invincible animation</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>✔</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>✔</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF006100"/>
+        <rFont val="新細明體"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(same as 3.)</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -232,7 +260,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -240,7 +268,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -254,7 +282,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0D0D0D"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -262,7 +290,7 @@
     <font>
       <sz val="15"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="等线"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -272,6 +300,21 @@
       <color theme="1" tint="4.9989318521683403E-2"/>
       <name val="Segoe UI Symbol"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Segoe UI Symbol"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -588,32 +631,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,12 +648,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,81 +655,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -720,59 +667,158 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1054,567 +1100,662 @@
   <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="17.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="9" style="2"/>
-    <col min="11" max="11" width="9" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="17.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="9" style="1"/>
+    <col min="11" max="11" width="9" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="54" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="20" t="s">
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="22"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="21"/>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="55" t="s">
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="24" t="s">
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="44"/>
-    </row>
-    <row r="3" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="3" t="s">
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="12"/>
+    </row>
+    <row r="3" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A3" s="6"/>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="55" t="s">
+      <c r="I3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="24" t="s">
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="44"/>
-    </row>
-    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="12"/>
+    </row>
+    <row r="4" spans="1:20" ht="15" thickBot="1">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="55" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="26" t="s">
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="27"/>
-      <c r="R4" s="27"/>
-      <c r="S4" s="51"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="29" t="s">
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="13"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="55" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="44"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" s="29" t="s">
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="12"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="55" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="44"/>
-    </row>
-    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="12"/>
+    </row>
+    <row r="7" spans="1:20" ht="15" thickBot="1">
+      <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="56"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="53" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="27" t="s">
         <v>31</v>
       </c>
       <c r="J7" s="28"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
-      <c r="M7" s="51"/>
-    </row>
-    <row r="8" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" s="58" t="s">
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="59"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="59"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="48"/>
-    </row>
-    <row r="11" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="52" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="52"/>
-      <c r="K11" s="52"/>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52"/>
-      <c r="N11" s="52"/>
-      <c r="O11" s="52"/>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="52"/>
-      <c r="S11" s="52"/>
+      <c r="J11" s="62"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="62"/>
+      <c r="N11" s="62"/>
+      <c r="O11" s="62"/>
+      <c r="P11" s="62"/>
+      <c r="Q11" s="62"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="62"/>
       <c r="T11"/>
     </row>
-    <row r="12" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="52"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52"/>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="52"/>
-      <c r="S12" s="52"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="47"/>
+      <c r="G12" s="47"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="62"/>
+      <c r="J12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
       <c r="T12"/>
     </row>
-    <row r="13" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I13" s="52"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="52"/>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52"/>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="52"/>
-      <c r="S13" s="52"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="62"/>
+      <c r="N13" s="62"/>
+      <c r="O13" s="62"/>
+      <c r="P13" s="62"/>
+      <c r="Q13" s="62"/>
+      <c r="R13" s="62"/>
+      <c r="S13" s="62"/>
       <c r="T13"/>
     </row>
-    <row r="14" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14">
+    <row r="14" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A14" s="6">
         <v>200</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="52"/>
+      <c r="B14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="62"/>
+      <c r="J14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="62"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="62"/>
+      <c r="P14" s="62"/>
+      <c r="Q14" s="62"/>
+      <c r="R14" s="62"/>
+      <c r="S14" s="62"/>
       <c r="T14"/>
     </row>
-    <row r="15" spans="1:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14">
+    <row r="15" spans="1:20" ht="14.25" customHeight="1">
+      <c r="A15" s="6">
         <v>250</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="52"/>
-      <c r="K15" s="52"/>
-      <c r="L15" s="52"/>
-      <c r="M15" s="52"/>
-      <c r="N15" s="52"/>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="52"/>
-      <c r="S15" s="52"/>
+      <c r="B15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="62"/>
+      <c r="J15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="62"/>
+      <c r="N15" s="62"/>
+      <c r="O15" s="62"/>
+      <c r="P15" s="62"/>
+      <c r="Q15" s="62"/>
+      <c r="R15" s="62"/>
+      <c r="S15" s="62"/>
       <c r="T15"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" s="14">
+    <row r="16" spans="1:20">
+      <c r="A16" s="6">
         <v>300</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="44"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="14">
+      <c r="B16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="6">
         <v>350</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="44"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="32"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="38" t="s">
+      <c r="B17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
-    </row>
-    <row r="20" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="30" t="s">
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="48"/>
+    </row>
+    <row r="20" spans="1:8" ht="18">
+      <c r="A20" s="34"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="34"/>
-      <c r="F20" s="30" t="s">
+      <c r="E20" s="53"/>
+      <c r="F20" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="32"/>
-    </row>
-    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="60" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1">
+      <c r="A21" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="45"/>
-      <c r="E21" s="46"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="48"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="60" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="45"/>
+      <c r="F21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" customHeight="1">
+      <c r="A22" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="61"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="46"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="48"/>
-    </row>
-    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="60" t="s">
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" s="45"/>
+      <c r="F22" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1">
+      <c r="A23" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="46"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="48"/>
-    </row>
-    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="60" t="s">
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="45"/>
+      <c r="F23" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="32"/>
+      <c r="H23" s="33"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" customHeight="1">
+      <c r="A24" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="48"/>
-    </row>
-    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="60" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="45"/>
+      <c r="F24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="32"/>
+      <c r="H24" s="33"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" customHeight="1">
+      <c r="A25" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="61"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="46"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="48"/>
-    </row>
-    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="60" t="s">
+      <c r="B25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="45"/>
+      <c r="F25" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="32"/>
+      <c r="H25" s="33"/>
+    </row>
+    <row r="26" spans="1:8" ht="30" customHeight="1">
+      <c r="A26" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
-    </row>
-    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="60" t="s">
+      <c r="B26" s="43"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E26" s="45"/>
+      <c r="F26" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="32"/>
+      <c r="H26" s="33"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" customHeight="1">
+      <c r="A27" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="46"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="48"/>
-    </row>
-    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="60" t="s">
+      <c r="B27" s="43"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="45"/>
+      <c r="F27" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="32"/>
+      <c r="H27" s="33"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" customHeight="1">
+      <c r="A28" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="61"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="48"/>
-    </row>
-    <row r="29" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
+      <c r="B28" s="43"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="45"/>
+      <c r="F28" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="32"/>
+      <c r="H28" s="33"/>
+    </row>
+    <row r="29" spans="1:8" ht="14.25" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" ht="18">
+      <c r="A30" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="41"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="36"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" thickBot="1">
+      <c r="A31" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="50"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="N1:S1"/>
-    <mergeCell ref="N2:R2"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="A19:H19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:H27"/>
     <mergeCell ref="F28:H28"/>
     <mergeCell ref="A30:H30"/>
@@ -1631,29 +1772,22 @@
     <mergeCell ref="A28:C28"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="N2:R2"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="I2:L2"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="I1:M1"/>
     <mergeCell ref="A12:H12"/>
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:H10"/>
     <mergeCell ref="I11:S15"/>
-    <mergeCell ref="A8:H8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>